<commit_message>
fixes to movement and calibration methods
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/mactaquac_calibration.xlsx
+++ b/bio_diversity/static/data_templates/mactaquac_calibration.xlsx
@@ -8,26 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoyelq\Desktop\Work\dm_apps\dm_apps\bio_diversity\static\data_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA03DD9-B3DC-4DC4-A5D5-72391CBD04A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184A105F-6B23-472A-BB21-73D8DF164706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="4065" windowWidth="23535" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tank" sheetId="3" r:id="rId1"/>
+    <sheet name="Trough" sheetId="5" r:id="rId2"/>
+    <sheet name="Drawer" sheetId="6" r:id="rId3"/>
+    <sheet name="Cup" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="17">
   <si>
     <t>Container Name:</t>
   </si>
   <si>
-    <t>Taged Fish in Container</t>
-  </si>
-  <si>
     <t>Current Values</t>
   </si>
   <si>
@@ -40,9 +40,6 @@
     <t>Group ID</t>
   </si>
   <si>
-    <t>Group</t>
-  </si>
-  <si>
     <t xml:space="preserve">New Group Count </t>
   </si>
   <si>
@@ -68,6 +65,15 @@
   </si>
   <si>
     <t>Optional. Was this a legitimate group that no longer exists? (Y/N)  Eg. Group was distributed.</t>
+  </si>
+  <si>
+    <t>Individuals or group</t>
+  </si>
+  <si>
+    <t>Stock details</t>
+  </si>
+  <si>
+    <t>ContainerLink</t>
   </si>
 </sst>
 </file>
@@ -1015,96 +1021,421 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="J2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:16" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" s="6" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3"/>
       <c r="K3"/>
       <c r="L3"/>
       <c r="M3"/>
       <c r="N3"/>
       <c r="O3"/>
+      <c r="P3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91D2664-AD29-4FE2-98AA-49CA0FFB3376}">
+  <dimension ref="A1:P3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A53552D-87D5-41CF-A0A8-BCDD8A4733A2}">
+  <dimension ref="A1:P3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A771E0BB-1487-485A-9772-E0FCFAE76358}">
+  <dimension ref="A1:P3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>